<commit_message>
First commit: upload project DACNTT
</commit_message>
<xml_diff>
--- a/data/DiaDiemDuLich/KhuDiemDuLich.xlsx
+++ b/data/DiaDiemDuLich/KhuDiemDuLich.xlsx
@@ -1,14 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
-    <sheet name="KhuDiemDuLich" sheetId="1" r:id="rId2"/>
+    <sheet name="KhuDiemDuLich" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -210,8 +224,7 @@
     <t>Điểm Du lịch Sinh Thái Dần Xây</t>
   </si>
   <si>
-    <t>1541 Rừng Sác, xã An Thới Đông, huyện Cần Giờ 
-</t>
+    <t>1541 Rừng Sác, xã An Thới Đông, huyện Cần Giờ</t>
   </si>
   <si>
     <t>0301074118-006</t>
@@ -319,22 +332,366 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -342,25 +699,805 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H31"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="61.5555555555556" customWidth="1"/>
+    <col min="3" max="3" width="74.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="11.7777777777778" customWidth="1"/>
+    <col min="5" max="5" width="19.7777777777778" customWidth="1"/>
+    <col min="6" max="6" width="12.8888888888889" customWidth="1"/>
+    <col min="7" max="7" width="15.6666666666667" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,7 +1523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -409,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -432,7 +1569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -455,7 +1592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -478,7 +1615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -501,7 +1638,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -524,7 +1661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -547,7 +1684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -570,7 +1707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -593,7 +1730,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -616,7 +1753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -639,7 +1776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -662,7 +1799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -685,7 +1822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -708,7 +1845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -731,7 +1868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -754,7 +1891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -777,7 +1914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -800,7 +1937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -823,7 +1960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -846,7 +1983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -869,7 +2006,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -892,7 +2029,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -915,7 +2052,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="2:7">
       <c r="B25" t="s">
         <v>81</v>
       </c>
@@ -935,7 +2072,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -958,7 +2095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -981,7 +2118,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -1004,7 +2141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>92</v>
       </c>
@@ -1027,7 +2164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -1050,7 +2187,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" ht="13" customHeight="1" spans="2:7">
       <c r="B31" t="s">
         <v>98</v>
       </c>
@@ -1071,5 +2208,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>